<commit_message>
made website responsive, added updated text
</commit_message>
<xml_diff>
--- a/data/Language holdingsF17.xlsx
+++ b/data/Language holdingsF17.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SIDL_Current/02_SIDL PROJECTS/1515_ELA/web/endangeredlanguages_csr/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SIDL_current/02_SIDL PROJECTS/1515_ELA/web/endangeredlanguages_csr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="460" windowWidth="27500" windowHeight="25740"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="27500" windowHeight="25740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="406">
   <si>
     <t>LANG</t>
   </si>
@@ -1239,6 +1239,12 @@
   </si>
   <si>
     <t>Armenian</t>
+  </si>
+  <si>
+    <t>top5sum</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -1281,11 +1287,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1298,6 +1306,849 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0909420384951881"/>
+          <c:y val="0.187465368912219"/>
+          <c:w val="0.889613517060367"/>
+          <c:h val="0.700054316127151"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.480720147732011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28049607529567</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0990203131515398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0906027044489147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.049160759371864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-1761036736"/>
+        <c:axId val="-1761034416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1761036736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1761034416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1761034416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1761036736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>946150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1098550</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1587,10 +2438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D211"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1599,7 +2450,7 @@
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1609,1150 +2460,1180 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>209818</v>
+      </c>
+      <c r="D2" s="4">
+        <f>SUM(C2:C6)</f>
+        <v>436466</v>
+      </c>
+      <c r="E2" s="5">
+        <f>(C2/D2)</f>
+        <v>0.48072014773201122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>122427</v>
+      </c>
+      <c r="E3" s="5">
+        <f>(C3/D2)</f>
+        <v>0.28049607529567022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43219</v>
+      </c>
+      <c r="E4" s="5">
+        <f>(C4/D2)</f>
+        <v>9.9020313151539863E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>39545</v>
+      </c>
+      <c r="E5" s="5">
+        <f>(C5/D2)</f>
+        <v>9.0602704448914689E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>21457</v>
+      </c>
+      <c r="E6" s="5">
+        <f>(C6/D2)</f>
+        <v>4.9160759371864017E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
-        <f>SUM(C7+C18+C23+C25+C45+C47+C55+C58+C68+C85+C100+C113+C117+C123+C156+C157+C164+C173+C174+C176+C193+C194)</f>
-        <v>4158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="2">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="2">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>11921</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3696</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>385</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>375</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>205</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3">
+        <v>6027</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>291</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5683</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>323</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>251</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>325</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4114</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="2">
-        <v>49</v>
+        <v>34</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3696</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="2">
-        <v>62</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3529</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3">
-        <v>12228</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>212</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C20" s="2">
-        <v>6</v>
+        <v>42</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2667</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>253</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C21" s="2">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2610</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>396</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2010</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="2">
-        <v>121</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1523</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>255</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1475</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="2">
-        <v>235</v>
+        <v>60</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1285</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="2">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1260</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>377</v>
+        <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1242</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>392</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1235</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="2">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1198</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="2">
-        <v>13</v>
+        <v>56</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1132</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>182</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2">
-        <v>10</v>
+        <v>976</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>327</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>328</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2">
-        <v>1</v>
+        <v>896</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="3">
-        <v>209818</v>
+        <v>66</v>
+      </c>
+      <c r="C33" s="2">
+        <v>790</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>317</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>318</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2">
-        <v>5</v>
+        <v>696</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>383</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>384</v>
+        <v>70</v>
       </c>
       <c r="C35" s="2">
-        <v>2</v>
+        <v>634</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>155</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2">
-        <v>18</v>
+        <v>599</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>277</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>278</v>
+        <v>74</v>
       </c>
       <c r="C37" s="2">
-        <v>2</v>
+        <v>563</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2">
-        <v>12</v>
+        <v>531</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2">
-        <v>24</v>
+        <v>511</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="C40" s="2">
-        <v>39</v>
+        <v>471</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="C41" s="2">
-        <v>11</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2">
-        <v>896</v>
+        <v>409</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C43" s="2">
-        <v>790</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>329</v>
+        <v>88</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>330</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2">
-        <v>1</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>88</v>
+        <v>403</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="2">
-        <v>343</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>192</v>
+        <v>91</v>
       </c>
       <c r="C46" s="2">
-        <v>8</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C47" s="2">
-        <v>408</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>214</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>215</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2">
-        <v>6</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>228</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>229</v>
+        <v>97</v>
       </c>
       <c r="C49" s="2">
-        <v>6</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>398</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>399</v>
+        <v>99</v>
       </c>
       <c r="C50" s="2">
-        <v>1</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
-        <v>257</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>258</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2">
-        <v>3</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C52" s="2">
-        <v>75</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="C53" s="2">
-        <v>20</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="C54" s="2">
-        <v>8</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C55" s="2">
-        <v>142</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>193</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2">
-        <v>8</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>185</v>
+        <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
       <c r="C57" s="2">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C58" s="2">
-        <v>263</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" s="3">
-        <v>21457</v>
+        <v>116</v>
+      </c>
+      <c r="C59" s="2">
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>259</v>
+        <v>117</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>260</v>
+        <v>118</v>
       </c>
       <c r="C60" s="2">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="C61" s="2">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>279</v>
+        <v>121</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>280</v>
+        <v>122</v>
       </c>
       <c r="C62" s="2">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>332</v>
+        <v>127</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>333</v>
+        <v>128</v>
       </c>
       <c r="C63" s="2">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
-        <v>261</v>
+        <v>123</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>262</v>
+        <v>124</v>
       </c>
       <c r="C64" s="2">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>211</v>
+        <v>126</v>
       </c>
       <c r="C65" s="2">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
-        <v>230</v>
+        <v>129</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>231</v>
+        <v>130</v>
       </c>
       <c r="C66" s="2">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="2" t="s">
-        <v>216</v>
+      <c r="A67" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>217</v>
+        <v>141</v>
       </c>
       <c r="C67" s="2">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="C68" s="2">
-        <v>124</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="3">
-        <v>11921</v>
+        <v>134</v>
+      </c>
+      <c r="C69" s="2">
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>334</v>
+        <v>143</v>
       </c>
       <c r="C70" s="2">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71" s="3">
-        <v>4901</v>
+        <v>132</v>
+      </c>
+      <c r="C71" s="2">
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C72" s="2">
-        <v>72</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
-        <v>281</v>
+        <v>139</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>282</v>
+        <v>140</v>
       </c>
       <c r="C73" s="2">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
-        <v>31</v>
+        <v>199</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="3">
-        <v>4114</v>
+        <v>200</v>
+      </c>
+      <c r="C74" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
-        <v>371</v>
+        <v>146</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>372</v>
+        <v>147</v>
       </c>
       <c r="C75" s="2">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C76" s="3">
-        <v>3529</v>
+        <v>145</v>
+      </c>
+      <c r="C76" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="C77" s="2">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="C78" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C79" s="3">
-        <v>6027</v>
+        <v>151</v>
+      </c>
+      <c r="C79" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
-        <v>390</v>
+        <v>152</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>391</v>
+        <v>153</v>
       </c>
       <c r="C80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="2">
+        <v>17</v>
+      </c>
+      <c r="D83">
+        <f>SUM(C87+C98+C103+C105+C125+C127+C135+C138+C148+C165+C180+C193+C197+C203+C236+C237+C244+C253+C254+C256+C273+C274)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="2">
         <v>13</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81" s="3">
-        <v>15290</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A82" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C82" s="3">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A83" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C83" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A84" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C84" s="2">
+    </row>
+    <row r="88" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C90" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A92" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A93" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C94" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C85" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C86" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C88" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A89" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" s="3">
-        <v>10424</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" s="3">
-        <v>5683</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A91" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C91" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A92" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C92" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C93" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A94" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="C94" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
-        <v>337</v>
+        <v>177</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>338</v>
+        <v>178</v>
       </c>
       <c r="C95" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
-        <v>339</v>
+        <v>181</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>340</v>
+        <v>182</v>
       </c>
       <c r="C96" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
-        <v>218</v>
+        <v>185</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="C97" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C98" s="3">
-        <v>43219</v>
+        <v>180</v>
+      </c>
+      <c r="C98" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
-        <v>379</v>
+        <v>183</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>380</v>
+        <v>184</v>
       </c>
       <c r="C99" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="C100" s="2">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C101" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
-        <v>381</v>
+        <v>203</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>382</v>
+        <v>204</v>
       </c>
       <c r="C102" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A103" s="2" t="s">
-        <v>61</v>
+      <c r="A103" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>62</v>
+        <v>207</v>
       </c>
       <c r="C103" s="2">
-        <v>976</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="C104" s="2">
-        <v>471</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C105" s="2">
         <v>8</v>
@@ -2760,175 +3641,175 @@
     </row>
     <row r="106" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="C106" s="2">
-        <v>511</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
-        <v>287</v>
+        <v>197</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>288</v>
+        <v>198</v>
       </c>
       <c r="C107" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>249</v>
+        <v>202</v>
       </c>
       <c r="C108" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="C109" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C110" s="3">
-        <v>2010</v>
+        <v>213</v>
+      </c>
+      <c r="C110" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="C111" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>322</v>
+        <v>229</v>
       </c>
       <c r="C112" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
-        <v>98</v>
+        <v>216</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>99</v>
+        <v>217</v>
       </c>
       <c r="C113" s="2">
-        <v>190</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="C114" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="C115" s="2">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="C116" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
-        <v>102</v>
+        <v>224</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
       </c>
       <c r="C117" s="2">
-        <v>143</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A118" s="2" t="s">
-        <v>341</v>
+      <c r="A118" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>342</v>
+        <v>226</v>
       </c>
       <c r="C118" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A119" s="2" t="s">
-        <v>57</v>
+      <c r="A119" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C119" s="3">
-        <v>1198</v>
+        <v>227</v>
+      </c>
+      <c r="C119" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="C120" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="C121" s="2">
         <v>5</v>
@@ -2936,153 +3817,153 @@
     </row>
     <row r="122" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="2" t="s">
-        <v>400</v>
+        <v>232</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>401</v>
+        <v>233</v>
       </c>
       <c r="C122" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2" t="s">
-        <v>96</v>
+        <v>246</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
       <c r="C123" s="2">
-        <v>227</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="C124" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="2" t="s">
-        <v>357</v>
+        <v>236</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>358</v>
+        <v>237</v>
       </c>
       <c r="C125" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
-        <v>220</v>
+        <v>310</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>221</v>
+        <v>311</v>
       </c>
       <c r="C126" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="2" t="s">
-        <v>75</v>
+        <v>238</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="C127" s="2">
-        <v>531</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A128" s="2" t="s">
-        <v>343</v>
+      <c r="A128" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>344</v>
+        <v>240</v>
       </c>
       <c r="C128" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
-        <v>345</v>
+        <v>241</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>346</v>
+        <v>242</v>
       </c>
       <c r="C129" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>298</v>
+        <v>249</v>
       </c>
       <c r="C130" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="2" t="s">
-        <v>142</v>
+        <v>244</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>143</v>
+        <v>245</v>
       </c>
       <c r="C131" s="2">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A132" s="2" t="s">
-        <v>347</v>
+      <c r="A132" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>348</v>
+        <v>243</v>
       </c>
       <c r="C132" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A133" s="2" t="s">
-        <v>299</v>
+      <c r="A133" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C133" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="2" t="s">
-        <v>37</v>
+        <v>308</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C134" s="3">
-        <v>3060</v>
+        <v>309</v>
+      </c>
+      <c r="C134" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C135" s="2">
         <v>3</v>
@@ -3090,32 +3971,32 @@
     </row>
     <row r="136" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>306</v>
+        <v>254</v>
       </c>
       <c r="C136" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
-        <v>53</v>
+        <v>255</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C137" s="3">
-        <v>1235</v>
+        <v>256</v>
+      </c>
+      <c r="C137" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="C138" s="2">
         <v>3</v>
@@ -3123,351 +4004,351 @@
     </row>
     <row r="139" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
-        <v>21</v>
+        <v>259</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C139" s="3">
-        <v>7756</v>
+        <v>260</v>
+      </c>
+      <c r="C139" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
-        <v>41</v>
+        <v>261</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C140" s="3">
-        <v>2667</v>
+        <v>262</v>
+      </c>
+      <c r="C140" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
-        <v>139</v>
+        <v>315</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>140</v>
+        <v>316</v>
       </c>
       <c r="C141" s="2">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>201</v>
+        <v>287</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="C142" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="C143" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>236</v>
+        <v>265</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="C144" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>51</v>
+        <v>275</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C145" s="3">
-        <v>1260</v>
+        <v>276</v>
+      </c>
+      <c r="C145" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
       <c r="C146" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="C147" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>9</v>
+        <v>271</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C148" s="3">
-        <v>39545</v>
+        <v>272</v>
+      </c>
+      <c r="C148" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
-        <v>165</v>
+        <v>273</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>166</v>
+        <v>274</v>
       </c>
       <c r="C149" s="2">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="C150" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2" t="s">
-        <v>45</v>
+        <v>383</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C151" s="3">
-        <v>1523</v>
+        <v>384</v>
+      </c>
+      <c r="C151" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="2" t="s">
-        <v>224</v>
+        <v>277</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
       <c r="C152" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="2" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="C153" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
       <c r="C154" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="2" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
       <c r="C155" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="2" t="s">
-        <v>112</v>
+        <v>285</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>113</v>
+        <v>286</v>
       </c>
       <c r="C156" s="2">
-        <v>77</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2" t="s">
-        <v>108</v>
+        <v>381</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>109</v>
+        <v>382</v>
       </c>
       <c r="C157" s="2">
-        <v>106</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="2" t="s">
-        <v>355</v>
+        <v>293</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>356</v>
+        <v>294</v>
       </c>
       <c r="C158" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2" t="s">
-        <v>183</v>
+        <v>295</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>184</v>
+        <v>296</v>
       </c>
       <c r="C159" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
-        <v>369</v>
+        <v>297</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>370</v>
+        <v>298</v>
       </c>
       <c r="C160" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>239</v>
+        <v>300</v>
       </c>
       <c r="C161" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="2" t="s">
-        <v>5</v>
+        <v>305</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C162" s="3">
-        <v>122427</v>
+        <v>306</v>
+      </c>
+      <c r="C162" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="C163" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="2" t="s">
-        <v>117</v>
+        <v>303</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="C164" s="2">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="2" t="s">
-        <v>359</v>
+        <v>313</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="C165" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A166" s="2" t="s">
-        <v>71</v>
+      <c r="A166" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>72</v>
+        <v>289</v>
       </c>
       <c r="C166" s="2">
-        <v>599</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A167" s="2" t="s">
-        <v>335</v>
+      <c r="A167" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>336</v>
+        <v>290</v>
       </c>
       <c r="C167" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A168" s="2" t="s">
-        <v>303</v>
+      <c r="A168" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C168" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A169" s="2" t="s">
-        <v>59</v>
+      <c r="A169" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C169" s="3">
-        <v>1285</v>
+        <v>312</v>
+      </c>
+      <c r="C169" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="2" t="s">
-        <v>361</v>
+        <v>319</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>362</v>
+        <v>320</v>
       </c>
       <c r="C170" s="2">
         <v>1</v>
@@ -3475,98 +4356,98 @@
     </row>
     <row r="171" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="2" t="s">
-        <v>271</v>
+        <v>385</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>272</v>
+        <v>386</v>
       </c>
       <c r="C171" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="2" t="s">
-        <v>203</v>
+        <v>375</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>204</v>
+        <v>376</v>
       </c>
       <c r="C172" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="2" t="s">
-        <v>92</v>
+        <v>323</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>93</v>
+        <v>324</v>
       </c>
       <c r="C173" s="2">
-        <v>243</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="2" t="s">
-        <v>121</v>
+        <v>325</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>122</v>
+        <v>326</v>
       </c>
       <c r="C174" s="2">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="2" t="s">
-        <v>47</v>
+        <v>396</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C175" s="3">
-        <v>1475</v>
+        <v>397</v>
+      </c>
+      <c r="C175" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="2" t="s">
-        <v>83</v>
+        <v>377</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>84</v>
+        <v>378</v>
       </c>
       <c r="C176" s="2">
-        <v>409</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="2" t="s">
-        <v>273</v>
+        <v>392</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>274</v>
+        <v>393</v>
       </c>
       <c r="C177" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="2" t="s">
-        <v>73</v>
+        <v>327</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>74</v>
+        <v>328</v>
       </c>
       <c r="C178" s="2">
-        <v>563</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="2" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="C179" s="2">
         <v>1</v>
@@ -3574,10 +4455,10 @@
     </row>
     <row r="180" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="2" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="C180" s="2">
         <v>1</v>
@@ -3585,10 +4466,10 @@
     </row>
     <row r="181" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="2" t="s">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="C181" s="2">
         <v>1</v>
@@ -3596,43 +4477,43 @@
     </row>
     <row r="182" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C182" s="3">
-        <v>1242</v>
+        <v>334</v>
+      </c>
+      <c r="C182" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="2" t="s">
-        <v>69</v>
+        <v>371</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>70</v>
+        <v>372</v>
       </c>
       <c r="C183" s="2">
-        <v>634</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="2" t="s">
-        <v>27</v>
+        <v>390</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C184" s="3">
-        <v>5322</v>
+        <v>391</v>
+      </c>
+      <c r="C184" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="2" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="C185" s="2">
         <v>1</v>
@@ -3640,21 +4521,21 @@
     </row>
     <row r="186" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="2" t="s">
-        <v>67</v>
+        <v>367</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>68</v>
+        <v>368</v>
       </c>
       <c r="C186" s="2">
-        <v>696</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="2" t="s">
-        <v>394</v>
+        <v>337</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>395</v>
+        <v>338</v>
       </c>
       <c r="C187" s="2">
         <v>1</v>
@@ -3662,233 +4543,233 @@
     </row>
     <row r="188" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="2" t="s">
-        <v>131</v>
+        <v>339</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>132</v>
+        <v>340</v>
       </c>
       <c r="C188" s="2">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="2" t="s">
-        <v>161</v>
+        <v>379</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>162</v>
+        <v>380</v>
       </c>
       <c r="C189" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="2" t="s">
-        <v>39</v>
+        <v>321</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C190" s="3">
-        <v>2610</v>
+        <v>322</v>
+      </c>
+      <c r="C190" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="2" t="s">
-        <v>129</v>
+        <v>341</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>130</v>
+        <v>342</v>
       </c>
       <c r="C191" s="2">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="2" t="s">
-        <v>313</v>
+        <v>400</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>314</v>
+        <v>401</v>
       </c>
       <c r="C192" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="2" t="s">
-        <v>110</v>
+        <v>357</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>111</v>
+        <v>358</v>
       </c>
       <c r="C193" s="2">
-        <v>94</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="2" t="s">
-        <v>403</v>
+        <v>343</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>87</v>
+        <v>344</v>
       </c>
       <c r="C194" s="2">
-        <v>326</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A195" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A195" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>141</v>
+        <v>346</v>
       </c>
       <c r="C195" s="2">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A196" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A196" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>158</v>
+        <v>348</v>
       </c>
       <c r="C196" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A197" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A197" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>169</v>
+        <v>352</v>
       </c>
       <c r="C197" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A198" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A198" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>176</v>
+        <v>354</v>
       </c>
       <c r="C198" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A199" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A199" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>207</v>
+        <v>356</v>
       </c>
       <c r="C199" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A200" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A200" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>226</v>
+        <v>370</v>
       </c>
       <c r="C200" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A201" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A201" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>227</v>
+        <v>360</v>
       </c>
       <c r="C201" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A202" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A202" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>240</v>
+        <v>336</v>
       </c>
       <c r="C202" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A203" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A203" s="2" t="s">
+        <v>361</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>243</v>
+        <v>362</v>
       </c>
       <c r="C203" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A204" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A204" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="C204" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A205" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A205" s="2" t="s">
+        <v>388</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>289</v>
+        <v>389</v>
       </c>
       <c r="C205" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A206" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A206" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>290</v>
+        <v>364</v>
       </c>
       <c r="C206" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A207" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A207" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>307</v>
+        <v>366</v>
       </c>
       <c r="C207" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="A208" s="2" t="e">
-        <v>#N/A</v>
+      <c r="A208" s="2" t="s">
+        <v>394</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>312</v>
+        <v>395</v>
       </c>
       <c r="C208" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -3925,9 +4806,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C211">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:D211">
+    <sortCondition descending="1" ref="C157"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>